<commit_message>
updated revision history for today
</commit_message>
<xml_diff>
--- a/doc/Revision History.xlsx
+++ b/doc/Revision History.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20730" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Revision History</t>
   </si>
@@ -32,12 +32,21 @@
   <si>
     <t>Author(s)</t>
   </si>
+  <si>
+    <t>Added use case diagrams, definition of done, vision and glossery</t>
+  </si>
+  <si>
+    <t>Added versioning conversions and use cases</t>
+  </si>
+  <si>
+    <t>Added product backlog, changed use cases, added estimates for tasks and sprint backlog</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +167,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -192,7 +201,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -368,27 +376,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="79.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -400,6 +408,30 @@
       </c>
       <c r="D2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="1">
+        <v>41235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="1">
+        <v>41239</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1">
+        <v>41240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -408,24 +440,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>